<commit_message>
Add background and fix Difficult mode
</commit_message>
<xml_diff>
--- a/Checklist-MidtermProject.xlsx
+++ b/Checklist-MidtermProject.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Midterm Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1930D8B4-11F8-4536-A6AE-FB0084A2CE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4776E0-E5F4-46F1-9697-A8A879F5AF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{830A96CF-C5D0-4BB6-BFBB-AFAD6E7AC5FE}"/>
+    <workbookView minimized="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{830A96CF-C5D0-4BB6-BFBB-AFAD6E7AC5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="For students" sheetId="2" r:id="rId1"/>
-    <sheet name="For graders" sheetId="3" r:id="rId2"/>
-    <sheet name="Rubric" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="For graders" sheetId="3" r:id="rId3"/>
+    <sheet name="Rubric" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="38">
   <si>
     <t>Generate board</t>
   </si>
@@ -412,33 +413,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -452,12 +429,36 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5445E293-FC48-4C88-9A8F-98A5A2EF1C38}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,13 +798,13 @@
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="I2" t="s">
         <v>36</v>
       </c>
@@ -812,31 +813,31 @@
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="19">
-        <v>201200001</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="11">
+        <v>201200001</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="11">
         <v>201200002</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -854,212 +855,212 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="C8" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D8" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D9" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D10" s="21">
+      <c r="C10" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D10" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D11" s="21">
+      <c r="C11" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D11" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D12" s="21">
+      <c r="C12" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D12" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D13" s="21">
+      <c r="C13" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D13" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="21">
-        <v>201200001</v>
-      </c>
-      <c r="D14" s="21">
+      <c r="C14" s="12">
+        <v>201200001</v>
+      </c>
+      <c r="D14" s="12">
         <v>201200002</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="12">
         <v>201200001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="12">
         <v>201200001</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="HTAlJl+oNUXx4J6hJaD7+rEp/ZRBu7WGtnozCWPNhgsrQ1VoJ0OnsAJesxpxx+pqb3NP2GHSeNxSog8xlTVKqQ==" saltValue="dP25V+BrDrkKMGnXnJgk9w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="6">
+    <mergeCell ref="A22:A28"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A22:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1067,11 +1068,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858E33C5-773D-44ED-A14F-73D80C853EC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C853CB2-E03D-4E3D-8BFF-ADEC30C2FB37}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,18 +1091,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="10" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J2" t="s">
@@ -1109,43 +1110,43 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="7">
         <f>'For students'!B3</f>
         <v>201200001</v>
       </c>
-      <c r="C3" s="13" t="str">
+      <c r="C3" s="19" t="str">
         <f>'For students'!C3</f>
         <v>Nguyễn Văn A</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="8">
         <f>SUMIF('For students'!$C$8:$D$14,$B$3,'For graders'!$C$8:$D$14)+SUMIF('For students'!$C$16:$C$20,$B$3,'For graders'!$C$16:$C$20)+SUMIF('For students'!$C$22:$C$28,$B$3,'For graders'!$C$22:$C$28)</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="7">
         <f>'For students'!B4</f>
         <v>201200002</v>
       </c>
-      <c r="C4" s="13" t="str">
+      <c r="C4" s="19" t="str">
         <f>'For students'!C4</f>
         <v>Nguyễn Văn B</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="8">
         <f>SUMIF('For students'!$C$8:$D$14,$B$4,'For graders'!$C$8:$D$14)+SUMIF('For students'!$C$16:$C$20,$B$4,'For graders'!$C$16:$C$20)+SUMIF('For students'!$C$22:$C$28,$B$4,'For graders'!$C$22:$C$28)</f>
         <v>0.5</v>
       </c>
@@ -1158,230 +1159,567 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D8" s="17">
-        <v>0.1</v>
+      <c r="C8" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <f xml:space="preserve"> SUM(C8:D14)</f>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="C9" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D10" s="17">
+      <c r="C10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="9">
         <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="C11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D11" s="9">
         <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D12" s="17">
+      <c r="C12" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="9">
         <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D13" s="17">
+      <c r="C13" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="9">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="C14" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="9">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D16" s="18"/>
+      <c r="C16" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D17" s="18"/>
+      <c r="C17" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D18" s="18"/>
+      <c r="C18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D19" s="18"/>
+      <c r="C19" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D20" s="18"/>
+      <c r="C20" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="18"/>
+      <c r="C22" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="10">
+        <f xml:space="preserve"> SUM(C22:C28)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="9">
         <v>0.15</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="9">
         <v>0.3</v>
       </c>
-      <c r="D24" s="18"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="9">
         <v>0.2</v>
       </c>
-      <c r="D25" s="18"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="9">
         <v>0.15</v>
       </c>
-      <c r="D26" s="18"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D27" s="18"/>
+      <c r="C27" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D28" s="18"/>
+      <c r="C28" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A22:A28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858E33C5-773D-44ED-A14F-73D80C853EC3}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
+    <col min="5" max="7" width="2.6328125" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7">
+        <f>'For students'!B3</f>
+        <v>201200001</v>
+      </c>
+      <c r="C3" s="19" t="str">
+        <f>'For students'!C3</f>
+        <v>Nguyễn Văn A</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="8">
+        <f>SUMIF('For students'!$C$8:$D$14,$B$3,'For graders'!$C$8:$D$14)+SUMIF('For students'!$C$16:$C$20,$B$3,'For graders'!$C$16:$C$20)+SUMIF('For students'!$C$22:$C$28,$B$3,'For graders'!$C$22:$C$28)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7">
+        <f>'For students'!B4</f>
+        <v>201200002</v>
+      </c>
+      <c r="C4" s="19" t="str">
+        <f>'For students'!C4</f>
+        <v>Nguyễn Văn B</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="8">
+        <f>SUMIF('For students'!$C$8:$D$14,$B$4,'For graders'!$C$8:$D$14)+SUMIF('For students'!$C$16:$C$20,$B$4,'For graders'!$C$16:$C$20)+SUMIF('For students'!$C$22:$C$28,$B$4,'For graders'!$C$22:$C$28)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
+      <c r="B28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D28" s="10"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="26u22Vw45Qp+wIPmm3hCIKB6C8UsLTKXdIlmUlCGwsYW/FEJqB0wef68s3zj1p+2PWHurMkHCbIS0gkvBEMRlg==" saltValue="NPjhZP647MDm195OjRYEfg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -1397,7 +1735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3864CD-EE60-4588-94D8-286FAA5AFEA0}">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -1429,7 +1767,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1443,7 +1781,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1455,7 +1793,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1467,7 +1805,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1479,7 +1817,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1491,7 +1829,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1503,7 +1841,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1515,7 +1853,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1526,7 +1864,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1873,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1544,7 +1882,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1553,7 +1891,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1562,7 +1900,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1573,7 +1911,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1920,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1591,7 +1929,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1600,7 +1938,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +1947,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1618,7 +1956,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>